<commit_message>
Hanle 'No Attachment' condition; Reset Excel font color after error
</commit_message>
<xml_diff>
--- a/email_map.xlsx
+++ b/email_map.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-83" yWindow="0" windowWidth="14566" windowHeight="17363" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TPC" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -43,6 +43,12 @@
       <u val="single"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="00000000"/>
+    </font>
+    <font>
+      <color rgb="00FF0000"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -65,10 +71,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,8 +423,8 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -471,6 +479,11 @@
           <t>redangelredux@hotmail.com</t>
         </is>
       </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>Sent on 08/04/2025 11:25</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -486,6 +499,11 @@
           <t>redangelredux@gmail.com</t>
         </is>
       </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>Sent on 08/04/2025 11:25</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -503,7 +521,12 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>accounting@sammynava.com</t>
+          <t>accounting</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Sent on 08/04/2025 11:25</t>
         </is>
       </c>
     </row>
@@ -515,7 +538,6 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C4" r:id="rId4"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId5"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C5" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D5" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -530,7 +552,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -585,9 +607,9 @@
           <t>redangelredux@hotmail.com</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Sent on 08/04/2025 10:54</t>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>Sent on 08/04/2025 11:28</t>
         </is>
       </c>
     </row>
@@ -605,9 +627,9 @@
           <t>redangelredux@gmail.com</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Sent on 08/04/2025 10:54</t>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>Error - No Attachement Found.</t>
         </is>
       </c>
     </row>
@@ -630,9 +652,9 @@
           <t>accounting@sammynava.com</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Sent on 08/04/2025 10:54</t>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Sent on 08/04/2025 11:28</t>
         </is>
       </c>
     </row>
@@ -783,8 +805,8 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -871,7 +893,7 @@
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>accounting@sammynava.com</t>
+          <t>accounting</t>
         </is>
       </c>
     </row>
@@ -893,7 +915,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C4" r:id="rId4"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B5" r:id="rId5"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C5" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D5" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D5" display="accounting@sammynava.com" r:id="rId7"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B6" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>